<commit_message>
added API that creates interaction
</commit_message>
<xml_diff>
--- a/docs/Twitter Clone API docs.xlsx
+++ b/docs/Twitter Clone API docs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturaronov/Desktop/Programming/react-fun/twitter-clone/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1991A9-90CE-7A44-8D4C-08715A755F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9843D3AD-6115-6749-B301-A59AE24081E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18860" yWindow="500" windowWidth="32340" windowHeight="20500" activeTab="1" xr2:uid="{5813C246-F6D0-3741-85BB-1B5F8FD0EE9D}"/>
+    <workbookView xWindow="16840" yWindow="5900" windowWidth="32340" windowHeight="20500" xr2:uid="{5813C246-F6D0-3741-85BB-1B5F8FD0EE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="142">
   <si>
     <t>Method</t>
   </si>
@@ -387,21 +387,6 @@
   </si>
   <si>
     <t>/api/my/profile/</t>
-  </si>
-  <si>
-    <t>{
-    "id": String,
-    "userName": String
-    "name": String,
-    "email": String
-    "bio": String,
-    "avatarImg": String,
-    "headerImg": String,
-    "location": String,
-    "website": String,
-    "dateOfBirth": String,
-    "joinDate": String
-}</t>
   </si>
   <si>
     <t>userName
@@ -427,6 +412,132 @@
   </si>
   <si>
     <t>/settings/password/index.jsx</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>/api/my/notifications/post</t>
+  </si>
+  <si>
+    <t>/api/my/notifications/post.jsx</t>
+  </si>
+  <si>
+    <t>useId
+content</t>
+  </si>
+  <si>
+    <t>{
+    "id": Int,
+    "userId": String,
+    "content": String,
+    "sendDate": Object,
+    "readDate": null,
+    "received": false
+}</t>
+  </si>
+  <si>
+    <t>{
+    "id": Int,
+    "userId": String,
+    "content": String,
+    "sendDate": Object,
+    "readDate": Object,
+    "received": true
+}</t>
+  </si>
+  <si>
+    <t>/api/my/notifications/read</t>
+  </si>
+  <si>
+    <t>/api/my/notifications/read.jsx</t>
+  </si>
+  <si>
+    <t>/api/my/posts</t>
+  </si>
+  <si>
+    <t>/api/my/posts.jsx</t>
+  </si>
+  <si>
+    <t>content
+mediaUrl
+postType
+postId</t>
+  </si>
+  <si>
+    <t>{
+    "id": Int,
+    "userId": String
+    "postId": Int,
+    "content": String,
+    "mediaUrl": String,
+    "date": Object,
+    "editDate": Object,
+    "postType": String
+}</t>
+  </si>
+  <si>
+    <t>/api/my/posts/:id</t>
+  </si>
+  <si>
+    <t>/api/my/posts/[id].jsx</t>
+  </si>
+  <si>
+    <t>401, 404, 406</t>
+  </si>
+  <si>
+    <t>/api/usersId/[id]/index.jsx</t>
+  </si>
+  <si>
+    <t>{
+    "id": String,
+    "userName": String
+    "name": String,
+    "email": String
+    "bio": String,
+    "avatarImg": String,
+    "headerImg": String,
+    "location": String,
+    "website": String,
+    "dateOfBirth": Object,
+    "joinDate": Object
+}</t>
+  </si>
+  <si>
+    <t>{
+    "id": String
+    "userName": String,
+    "name": String,
+    "email": String,
+    "bio": String,
+    "avatarImg": String
+    "headerImg": String,
+    "location": String,
+    "website": String,
+    "dateOfBirth": Object,
+    "joinDate": Object
+}</t>
+  </si>
+  <si>
+    <t>/api/usersId</t>
+  </si>
+  <si>
+    <t>/api/users/[username]/index.jsx</t>
+  </si>
+  <si>
+    <t>/api/users/:username/following</t>
+  </si>
+  <si>
+    <t>/api/users/:username</t>
+  </si>
+  <si>
+    <t>/api/users/:username/following.jsx</t>
+  </si>
+  <si>
+    <t>/api/users/:username/followers</t>
+  </si>
+  <si>
+    <t>/api/users/:username/followers.jsx</t>
   </si>
 </sst>
 </file>
@@ -1060,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D93CE9B-366E-3045-AC1D-91F5BBC2A031}">
   <dimension ref="A1:BP50"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="110" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1316,7 @@
         <v>60</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>18</v>
@@ -1225,10 +1336,10 @@
         <v>102</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="G8" s="34" t="s">
         <v>18</v>
@@ -1242,6 +1353,214 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="221" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="50" spans="68:68" x14ac:dyDescent="0.2">
       <c r="BP50" s="2" t="s">
@@ -1261,7 +1580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B0B0AB-285A-984C-9A11-66BA095C2B90}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
+    <sheetView zoomScale="132" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1342,13 +1661,13 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1362,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1376,7 +1695,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed follows-likes-bookmarks into interactions
</commit_message>
<xml_diff>
--- a/docs/Twitter Clone API docs.xlsx
+++ b/docs/Twitter Clone API docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arturaronov/Desktop/Programming/react-fun/twitter-clone/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF200FDF-C58E-BD4E-8CEB-E554DE072205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3A9EA2-3310-A844-AF92-B215C419C6B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16840" yWindow="5900" windowWidth="32340" windowHeight="20500" xr2:uid="{5813C246-F6D0-3741-85BB-1B5F8FD0EE9D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="149">
   <si>
     <t>Method</t>
   </si>
@@ -540,16 +540,43 @@
     <t>/api/users/:username/followers.jsx</t>
   </si>
   <si>
-    <t>/api/my/follows-likes-bookmarks</t>
-  </si>
-  <si>
-    <t>/api/my/follows-likes-bookmarks.jsx</t>
-  </si>
-  <si>
     <t>/api/my/interaction</t>
   </si>
   <si>
     <t>/api/my/interaction.jsx</t>
+  </si>
+  <si>
+    <t>{
+    "id": Int,
+    "postId": Int,
+    "postUserId": String,
+    "interactionUserId": String,
+    "date": Object,
+    "actionType": String
+}</t>
+  </si>
+  <si>
+    <t>postId
+interactionUserId
+actionType</t>
+  </si>
+  <si>
+    <t>/api/my/interactions.jsx</t>
+  </si>
+  <si>
+    <t>[
+    {
+        "id": Int,
+        "postId": Int,
+        "postUserId": String,
+        "interactionUserId": String,
+        "date": Object,
+        "actionType": String
+    }
+]</t>
+  </si>
+  <si>
+    <t>/api/my/interactions</t>
   </si>
 </sst>
 </file>
@@ -1183,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D93CE9B-366E-3045-AC1D-91F5BBC2A031}">
   <dimension ref="A1:BP50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="110" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1574,39 +1601,60 @@
       <c r="F21" s="6"/>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="170" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>147</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>145</v>
       </c>
+      <c r="F23" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="G23" s="34" t="s">
-        <v>131</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="50" spans="68:68" x14ac:dyDescent="0.2">
       <c r="BP50" s="2" t="s">

</xml_diff>